<commit_message>
added factor for carbon debt
into biofuel (biomass product) production process
</commit_message>
<xml_diff>
--- a/data/shared/shared_calcs.xlsx
+++ b/data/shared/shared_calcs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\BlackBlox\data\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25654CF8-2F7E-E545-A235-CA21DCBE6A62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="460" windowWidth="21380" windowHeight="17540" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="465" windowWidth="21375" windowHeight="17535" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="1" r:id="rId1"/>
@@ -32,7 +31,7 @@
     <sheet name="CO2 Compress" sheetId="24" r:id="rId17"/>
     <sheet name="CO2 Storage" sheetId="14" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1524" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="223">
   <si>
     <t>combustion</t>
   </si>
@@ -702,12 +701,27 @@
   </si>
   <si>
     <t>CO2 losses</t>
+  </si>
+  <si>
+    <t>carbon debt</t>
+  </si>
+  <si>
+    <t>embodied CO2</t>
+  </si>
+  <si>
+    <t>CO2 removal</t>
+  </si>
+  <si>
+    <t>debt CO2</t>
+  </si>
+  <si>
+    <t>carbon debt factor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -906,8 +920,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1218,21 +1232,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -1264,7 +1278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1287,7 +1301,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1324,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1333,7 +1347,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>121</v>
       </c>
@@ -1356,7 +1370,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>121</v>
       </c>
@@ -1376,7 +1390,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>121</v>
       </c>
@@ -1399,7 +1413,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>121</v>
       </c>
@@ -1419,7 +1433,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1442,7 +1456,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1462,7 +1476,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>179</v>
       </c>
@@ -1482,7 +1496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -1508,21 +1522,21 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="R2" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1554,7 +1568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>193</v>
       </c>
@@ -1577,7 +1591,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1600,7 +1614,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>19</v>
       </c>
@@ -1617,7 +1631,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1640,7 +1654,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="33" t="s">
         <v>93</v>
@@ -1659,7 +1673,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1682,7 +1696,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
         <v>193</v>
       </c>
@@ -1702,7 +1716,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>179</v>
       </c>
@@ -1722,7 +1736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>195</v>
@@ -1738,6 +1752,49 @@
       </c>
       <c r="F10" s="31" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -1746,20 +1803,20 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:J25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="4" max="4" width="19.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1791,7 +1848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>145</v>
       </c>
@@ -1817,7 +1874,7 @@
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1841,7 +1898,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="21" t="s">
         <v>141</v>
@@ -1863,7 +1920,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="21" t="s">
         <v>141</v>
@@ -1885,7 +1942,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="10" t="s">
         <v>93</v>
@@ -1905,7 +1962,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="10" t="s">
         <v>54</v>
@@ -1925,7 +1982,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1948,7 +2005,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
@@ -1965,7 +2022,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -1988,7 +2045,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>167</v>
       </c>
@@ -2011,7 +2068,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -2034,7 +2091,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -2057,7 +2114,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
         <v>144</v>
       </c>
@@ -2077,7 +2134,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>150</v>
       </c>
@@ -2100,7 +2157,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="28" t="s">
         <v>177</v>
@@ -2119,7 +2176,7 @@
       </c>
       <c r="G16" s="23"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>146</v>
       </c>
@@ -2145,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
         <v>144</v>
       </c>
@@ -2162,7 +2219,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
         <v>159</v>
       </c>
@@ -2185,7 +2242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>73</v>
       </c>
@@ -2208,7 +2265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>172</v>
       </c>
@@ -2231,7 +2288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>173</v>
       </c>
@@ -2254,7 +2311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
         <v>162</v>
       </c>
@@ -2277,7 +2334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>179</v>
       </c>
@@ -2297,7 +2354,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>179</v>
       </c>
@@ -2315,6 +2372,49 @@
       </c>
       <c r="F25" s="31" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>221</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2323,16 +2423,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -2366,7 +2466,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>75</v>
       </c>
@@ -2394,7 +2494,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -2422,7 +2522,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -2450,7 +2550,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -2476,7 +2576,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -2502,7 +2602,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>179</v>
       </c>
@@ -2534,26 +2634,26 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -2585,7 +2685,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
@@ -2605,7 +2705,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2625,7 +2725,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>19</v>
       </c>
@@ -2645,7 +2745,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>179</v>
       </c>
@@ -2665,7 +2765,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -2691,16 +2791,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -2732,7 +2832,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="35" t="s">
         <v>111</v>
@@ -2756,7 +2856,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="35" t="s">
         <v>54</v>
@@ -2780,7 +2880,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="35" t="s">
         <v>111</v>
@@ -2804,7 +2904,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>93</v>
       </c>
@@ -2824,7 +2924,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
@@ -2847,7 +2947,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>72</v>
       </c>
@@ -2868,7 +2968,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>179</v>
       </c>
@@ -2888,7 +2988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>179</v>
       </c>
@@ -2914,26 +3014,26 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -2965,7 +3065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>106</v>
       </c>
@@ -2991,7 +3091,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>106</v>
       </c>
@@ -3014,7 +3114,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>107</v>
       </c>
@@ -3034,7 +3134,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>107</v>
       </c>
@@ -3054,7 +3154,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>72</v>
       </c>
@@ -3077,7 +3177,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>19</v>
       </c>
@@ -3094,7 +3194,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="33" t="s">
         <v>216</v>
       </c>
@@ -3114,7 +3214,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>111</v>
       </c>
@@ -3131,7 +3231,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>150</v>
       </c>
@@ -3154,7 +3254,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="28" t="s">
         <v>177</v>
@@ -3179,26 +3279,26 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9507DF2-D8F8-0B40-8678-5267C4E8FA82}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -3230,7 +3330,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>106</v>
       </c>
@@ -3256,7 +3356,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>106</v>
       </c>
@@ -3279,7 +3379,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>107</v>
       </c>
@@ -3299,7 +3399,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>107</v>
       </c>
@@ -3319,7 +3419,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>72</v>
       </c>
@@ -3342,7 +3442,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
         <v>19</v>
       </c>
@@ -3359,7 +3459,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="33" t="s">
         <v>216</v>
       </c>
@@ -3379,7 +3479,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>111</v>
       </c>
@@ -3396,7 +3496,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>150</v>
       </c>
@@ -3419,7 +3519,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="28" t="s">
         <v>177</v>
@@ -3444,16 +3544,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB37DD3A-244E-E941-BEB9-43BF9377FFBD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -3485,7 +3585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>106</v>
       </c>
@@ -3511,7 +3611,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="35" t="s">
         <v>216</v>
       </c>
@@ -3531,7 +3631,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>72</v>
       </c>
@@ -3554,7 +3654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="15" t="s">
         <v>19</v>
@@ -3579,22 +3679,22 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -3626,7 +3726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>119</v>
       </c>
@@ -3646,7 +3746,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>119</v>
       </c>
@@ -3666,7 +3766,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>156</v>
       </c>
@@ -3686,7 +3786,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -3703,7 +3803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>119</v>
       </c>
@@ -3723,7 +3823,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>175</v>
       </c>
@@ -3740,7 +3840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>156</v>
       </c>
@@ -3766,16 +3866,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3807,7 +3907,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -3830,7 +3930,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -3853,7 +3953,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3879,7 +3979,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -3905,7 +4005,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -3928,7 +4028,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -3948,7 +4048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>179</v>
       </c>
@@ -3969,7 +4069,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>179</v>
       </c>
@@ -3996,20 +4096,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -4041,7 +4141,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4064,7 +4164,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4084,7 +4184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4107,7 +4207,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -4130,7 +4230,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4150,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -4170,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
@@ -4193,7 +4293,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
@@ -4216,7 +4316,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4239,7 +4339,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -4259,7 +4359,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -4279,7 +4379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>179</v>
       </c>
@@ -4305,20 +4405,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -4350,7 +4450,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4373,7 +4473,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4393,7 +4493,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4416,7 +4516,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -4439,7 +4539,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4459,7 +4559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -4479,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -4502,7 +4602,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -4525,7 +4625,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4548,7 +4648,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -4568,7 +4668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -4588,7 +4688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>179</v>
       </c>
@@ -4614,20 +4714,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -4659,7 +4759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -4682,7 +4782,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -4705,7 +4805,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>52</v>
       </c>
@@ -4728,7 +4828,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
@@ -4748,7 +4848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
@@ -4771,7 +4871,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>52</v>
       </c>
@@ -4794,7 +4894,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -4814,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -4834,7 +4934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>132</v>
       </c>
@@ -4857,7 +4957,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>132</v>
       </c>
@@ -4877,7 +4977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>132</v>
       </c>
@@ -4900,7 +5000,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>132</v>
       </c>
@@ -4923,7 +5023,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>132</v>
       </c>
@@ -4943,7 +5043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>132</v>
       </c>
@@ -4964,7 +5064,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>132</v>
       </c>
@@ -4988,7 +5088,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -5011,7 +5111,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -5031,7 +5131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -5054,7 +5154,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>10</v>
       </c>
@@ -5074,7 +5174,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
@@ -5100,7 +5200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
@@ -5126,7 +5226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>179</v>
       </c>
@@ -5146,7 +5246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>179</v>
       </c>
@@ -5172,20 +5272,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="A7:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -5217,7 +5317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>139</v>
       </c>
@@ -5240,7 +5340,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>155</v>
       </c>
@@ -5260,7 +5360,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>19</v>
       </c>
@@ -5277,7 +5377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -5300,7 +5400,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>73</v>
       </c>
@@ -5317,7 +5417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -5340,7 +5440,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -5363,7 +5463,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -5386,7 +5486,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -5406,7 +5506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -5426,7 +5526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>142</v>
       </c>
@@ -5452,7 +5552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>179</v>
       </c>
@@ -5472,7 +5572,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>179</v>
       </c>
@@ -5499,21 +5599,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -5545,7 +5645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -5568,7 +5668,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -5591,7 +5691,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
@@ -5618,7 +5718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -5645,7 +5745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>64</v>
       </c>
@@ -5668,7 +5768,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>64</v>
       </c>
@@ -5688,7 +5788,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>64</v>
       </c>
@@ -5711,7 +5811,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>64</v>
       </c>
@@ -5734,7 +5834,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>64</v>
       </c>
@@ -5754,7 +5854,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
@@ -5774,7 +5874,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
@@ -5797,7 +5897,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -5818,7 +5918,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -5841,7 +5941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -5861,7 +5961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>82</v>
       </c>
@@ -5884,7 +5984,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>82</v>
       </c>
@@ -5904,7 +6004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>179</v>
       </c>
@@ -5924,7 +6024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>179</v>
       </c>
@@ -5950,20 +6050,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -5995,7 +6095,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6018,7 +6118,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>33</v>
       </c>
@@ -6038,7 +6138,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -6061,7 +6161,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>126</v>
       </c>
@@ -6084,7 +6184,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>104</v>
       </c>
@@ -6107,7 +6207,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>138</v>
       </c>
@@ -6130,7 +6230,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -6153,7 +6253,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -6170,7 +6270,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -6193,7 +6293,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>19</v>
       </c>
@@ -6210,7 +6310,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -6230,7 +6330,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>129</v>
       </c>
@@ -6250,7 +6350,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>129</v>
       </c>
@@ -6270,7 +6370,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>54</v>
       </c>
@@ -6287,7 +6387,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -6304,7 +6404,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -6327,7 +6427,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>73</v>
       </c>
@@ -6344,7 +6444,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>179</v>
       </c>
@@ -6364,7 +6464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>179</v>
       </c>
@@ -6390,16 +6490,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -6422,7 +6522,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>16</v>
       </c>
@@ -6445,7 +6545,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="22" t="s">
         <v>33</v>
@@ -6466,7 +6566,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="27" t="s">
         <v>147</v>
@@ -6485,7 +6585,7 @@
       </c>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="27" t="s">
         <v>176</v>
@@ -6504,7 +6604,7 @@
       </c>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -6527,7 +6627,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>19</v>
       </c>
@@ -6544,7 +6644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -6567,7 +6667,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>73</v>
       </c>
@@ -6584,7 +6684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -6607,7 +6707,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
         <v>38</v>
@@ -6626,7 +6726,7 @@
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -6646,7 +6746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>187</v>
@@ -6664,7 +6764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>213</v>
       </c>
@@ -6684,7 +6784,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="35" t="s">
         <v>214</v>
       </c>

</xml_diff>